<commit_message>
basic plot of I vs V
</commit_message>
<xml_diff>
--- a/Lab4 - Photoelectric Effect/Experiment .xlsx
+++ b/Lab4 - Photoelectric Effect/Experiment .xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/t905k768_home_ku_edu/Documents/PHSX 616/GitHub/PHSX616/Lab4 - Photoelectric Effect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="690" documentId="8_{815DA9DA-EEA1-4F15-BC6C-79DBF2B13E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFDDA76D-C938-446C-B411-0A26979F88C0}"/>
+  <xr:revisionPtr revIDLastSave="691" documentId="8_{815DA9DA-EEA1-4F15-BC6C-79DBF2B13E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A981E147-6510-4C2B-BCF9-97D10FD405E6}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{B4EC2E35-03E0-4218-B9E1-B03C228EF9DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B4EC2E35-03E0-4218-B9E1-B03C228EF9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="1-ap2_t1" sheetId="2" r:id="rId2"/>
-    <sheet name="1-ap2_t2" sheetId="3" r:id="rId3"/>
+    <sheet name="2-ap2_t2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2156,7 +2156,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$A$2:$A$22</c:f>
+              <c:f>'2-ap2_t2'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2228,7 +2228,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$B$2:$B$22</c:f>
+              <c:f>'2-ap2_t2'!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2334,7 +2334,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$A$2:$A$22</c:f>
+              <c:f>'2-ap2_t2'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2406,7 +2406,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$C$2:$C$22</c:f>
+              <c:f>'2-ap2_t2'!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2512,7 +2512,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$A$2:$A$22</c:f>
+              <c:f>'2-ap2_t2'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2584,7 +2584,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$D$2:$D$22</c:f>
+              <c:f>'2-ap2_t2'!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2690,7 +2690,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$A$2:$A$22</c:f>
+              <c:f>'2-ap2_t2'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2762,7 +2762,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$E$2:$E$22</c:f>
+              <c:f>'2-ap2_t2'!$E$2:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2868,7 +2868,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$A$2:$A$22</c:f>
+              <c:f>'2-ap2_t2'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -2940,7 +2940,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1-ap2_t2'!$F$2:$F$22</c:f>
+              <c:f>'2-ap2_t2'!$F$2:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -4730,7 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B194152-B288-4AFE-BC10-02D24C820687}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:B28"/>
     </sheetView>
   </sheetViews>
@@ -5911,8 +5911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5BF6FE-8556-4231-A2E8-901300CB79CB}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>